<commit_message>
arreglo carga masiva para usuarios, cambio los mensajes de error y agrego validacion para los datos
</commit_message>
<xml_diff>
--- a/administrador/static/administrador/plantillas/plantilla_usuarios.xlsx
+++ b/administrador/static/administrador/plantillas/plantilla_usuarios.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bayron\OneDrive\Escritorio\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12330"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28770" windowHeight="11700"/>
   </bookViews>
   <sheets>
-    <sheet name="Usuarios" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -52,11 +52,16 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ h:mm:ss"/>
-  </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -72,12 +77,27 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -86,7 +106,9 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -105,7 +127,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -147,7 +169,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -179,9 +201,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -213,6 +236,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -389,50 +413,44 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:I1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="L7" sqref="L7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="4" max="4" width="17.140625" bestFit="1" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="D2" s="1"/>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>